<commit_message>
update of miniWECC split plus weekly
</commit_message>
<xml_diff>
--- a/excel/miniWECC_split/miniWECC_split.xlsx
+++ b/excel/miniWECC_split/miniWECC_split.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
   <si>
     <t xml:space="preserve">BCH-G1      </t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>(Mbase &gt;= 4000 MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- no gov</t>
   </si>
 </sst>
 </file>
@@ -763,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P83"/>
+  <dimension ref="B1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>129</v>
       </c>
@@ -1998,6 +2004,9 @@
       <c r="D49" t="s">
         <v>131</v>
       </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
       <c r="G49" t="s">
         <v>134</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1</v>
       </c>
@@ -2015,11 +2024,29 @@
       <c r="D50">
         <v>1</v>
       </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
       <c r="G50" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50" t="s">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>3</v>
       </c>
@@ -2029,8 +2056,11 @@
       <c r="D51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>5</v>
       </c>
@@ -2040,8 +2070,26 @@
       <c r="D52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>17</v>
+      </c>
+      <c r="O52" t="s">
+        <v>16</v>
+      </c>
+      <c r="P52">
+        <v>7</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+      <c r="S52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>9</v>
       </c>
@@ -2051,11 +2099,29 @@
       <c r="D53">
         <v>4</v>
       </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
       <c r="G53" t="s">
+        <v>139</v>
+      </c>
+      <c r="N53">
+        <v>23</v>
+      </c>
+      <c r="O53" t="s">
+        <v>22</v>
+      </c>
+      <c r="P53">
+        <v>10</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>12</v>
       </c>
@@ -2065,8 +2131,26 @@
       <c r="D54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>118</v>
+      </c>
+      <c r="O54" t="s">
+        <v>130</v>
+      </c>
+      <c r="P54">
+        <v>34</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>14</v>
       </c>
@@ -2076,8 +2160,11 @@
       <c r="D55">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>17</v>
       </c>
@@ -2087,8 +2174,8 @@
       <c r="D56">
         <v>7</v>
       </c>
-      <c r="F56" t="s">
-        <v>133</v>
+      <c r="F56">
+        <v>1</v>
       </c>
       <c r="G56" t="s">
         <v>135</v>
@@ -2096,8 +2183,11 @@
       <c r="H56" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>19</v>
       </c>
@@ -2107,11 +2197,14 @@
       <c r="D57">
         <v>8</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>22</v>
       </c>
@@ -2121,11 +2214,14 @@
       <c r="D58">
         <v>9</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="I58" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>23</v>
       </c>
@@ -2135,14 +2231,17 @@
       <c r="D59">
         <v>10</v>
       </c>
-      <c r="F59" t="s">
-        <v>133</v>
+      <c r="F59">
+        <v>1</v>
       </c>
       <c r="G59" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>25</v>
       </c>
@@ -2152,11 +2251,14 @@
       <c r="D60">
         <v>11</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>27</v>
       </c>
@@ -2166,8 +2268,26 @@
       <c r="D61">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>68</v>
+      </c>
+      <c r="O61" t="s">
+        <v>67</v>
+      </c>
+      <c r="P61">
+        <v>29</v>
+      </c>
+      <c r="R61">
+        <v>2</v>
+      </c>
+      <c r="S61" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>30</v>
       </c>
@@ -2177,8 +2297,26 @@
       <c r="D62">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <v>71</v>
+      </c>
+      <c r="O62" t="s">
+        <v>67</v>
+      </c>
+      <c r="P62">
+        <v>30</v>
+      </c>
+      <c r="R62">
+        <v>2</v>
+      </c>
+      <c r="S62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>32</v>
       </c>
@@ -2188,8 +2326,11 @@
       <c r="D63">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>34</v>
       </c>
@@ -2199,8 +2340,11 @@
       <c r="D64">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>37</v>
       </c>
@@ -2210,8 +2354,11 @@
       <c r="D65">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>39</v>
       </c>
@@ -2221,8 +2368,11 @@
       <c r="D66">
         <v>17</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>41</v>
       </c>
@@ -2232,11 +2382,14 @@
       <c r="D67">
         <v>18</v>
       </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
       <c r="G67" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>45</v>
       </c>
@@ -2246,8 +2399,11 @@
       <c r="D68">
         <v>19</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>47</v>
       </c>
@@ -2257,8 +2413,11 @@
       <c r="D69">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>48</v>
       </c>
@@ -2268,11 +2427,29 @@
       <c r="D70">
         <v>21</v>
       </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
       <c r="G70" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>41</v>
+      </c>
+      <c r="O70" t="s">
+        <v>40</v>
+      </c>
+      <c r="P70">
+        <v>18</v>
+      </c>
+      <c r="R70">
+        <v>3</v>
+      </c>
+      <c r="S70" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>51</v>
       </c>
@@ -2282,8 +2459,26 @@
       <c r="D71">
         <v>22</v>
       </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>3</v>
+      </c>
+      <c r="N71">
+        <v>48</v>
+      </c>
+      <c r="O71" t="s">
+        <v>47</v>
+      </c>
+      <c r="P71">
+        <v>21</v>
+      </c>
+      <c r="R71">
+        <v>3</v>
+      </c>
+      <c r="S71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>53</v>
       </c>
@@ -2293,8 +2488,26 @@
       <c r="D72">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>3</v>
+      </c>
+      <c r="N72">
+        <v>59</v>
+      </c>
+      <c r="O72" t="s">
+        <v>58</v>
+      </c>
+      <c r="P72">
+        <v>25</v>
+      </c>
+      <c r="R72">
+        <v>3</v>
+      </c>
+      <c r="S72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>58</v>
       </c>
@@ -2304,8 +2517,11 @@
       <c r="D73">
         <v>24</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>59</v>
       </c>
@@ -2315,11 +2531,29 @@
       <c r="D74">
         <v>25</v>
       </c>
+      <c r="F74">
+        <v>3</v>
+      </c>
       <c r="G74" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>65</v>
+      </c>
+      <c r="O74" t="s">
+        <v>64</v>
+      </c>
+      <c r="P74">
+        <v>28</v>
+      </c>
+      <c r="R74">
+        <v>3</v>
+      </c>
+      <c r="S74" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>60</v>
       </c>
@@ -2329,11 +2563,14 @@
       <c r="D75">
         <v>26</v>
       </c>
+      <c r="F75">
+        <v>3</v>
+      </c>
       <c r="G75" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>62</v>
       </c>
@@ -2343,14 +2580,17 @@
       <c r="D76">
         <v>27</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76">
+        <v>3</v>
+      </c>
+      <c r="G76" t="s">
+        <v>138</v>
+      </c>
+      <c r="I76" t="s">
         <v>132</v>
       </c>
-      <c r="G76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>65</v>
       </c>
@@ -2360,11 +2600,14 @@
       <c r="D77">
         <v>28</v>
       </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
       <c r="G77" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>68</v>
       </c>
@@ -2374,11 +2617,14 @@
       <c r="D78">
         <v>29</v>
       </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
       <c r="G78" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>71</v>
       </c>
@@ -2388,11 +2634,14 @@
       <c r="D79">
         <v>30</v>
       </c>
+      <c r="F79">
+        <v>2</v>
+      </c>
       <c r="G79" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>74</v>
       </c>
@@ -2401,6 +2650,9 @@
       </c>
       <c r="D80">
         <v>31</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -2413,6 +2665,9 @@
       <c r="D81">
         <v>32</v>
       </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82">
@@ -2424,6 +2679,9 @@
       <c r="D82">
         <v>33</v>
       </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83">
@@ -2434,6 +2692,9 @@
       </c>
       <c r="D83">
         <v>34</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
       </c>
       <c r="G83" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
update of miniwecc split info
</commit_message>
<xml_diff>
--- a/excel/miniWECC_split/miniWECC_split.xlsx
+++ b/excel/miniWECC_split/miniWECC_split.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="146">
   <si>
     <t xml:space="preserve">BCH-G1      </t>
   </si>
@@ -444,6 +444,24 @@
   </si>
   <si>
     <t xml:space="preserve"> -- no gov</t>
+  </si>
+  <si>
+    <t>Gens for ramping</t>
+  </si>
+  <si>
+    <t>Area 1:</t>
+  </si>
+  <si>
+    <t>Area 2:</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>mbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +400 MW over 1200 seconds (20 minutes)</t>
   </si>
 </sst>
 </file>
@@ -771,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1240,7 +1258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1269,7 +1287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1298,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1327,7 +1345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1356,7 +1374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
@@ -1385,7 +1403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
@@ -1472,7 +1490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
@@ -1501,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
@@ -1530,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
@@ -1559,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
@@ -1588,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
@@ -1617,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
@@ -1645,8 +1663,11 @@
       <c r="L31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>
@@ -1675,7 +1696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>30</v>
       </c>
@@ -1703,8 +1724,17 @@
       <c r="L33" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>140</v>
+      </c>
+      <c r="P33" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>31</v>
       </c>
@@ -1732,8 +1762,20 @@
       <c r="L34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>141</v>
+      </c>
+      <c r="O34">
+        <v>25</v>
+      </c>
+      <c r="P34">
+        <v>2256</v>
+      </c>
+      <c r="Q34">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>32</v>
       </c>
@@ -1761,8 +1803,20 @@
       <c r="L35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>142</v>
+      </c>
+      <c r="O35">
+        <v>74</v>
+      </c>
+      <c r="P35">
+        <v>1776</v>
+      </c>
+      <c r="Q35">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>33</v>
       </c>
@@ -1791,7 +1845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>34</v>
       </c>
@@ -1820,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>35</v>
       </c>
@@ -1849,7 +1903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>36</v>
       </c>
@@ -1878,7 +1932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>37</v>
       </c>
@@ -1907,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>38</v>
       </c>
@@ -1936,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>39</v>
       </c>
@@ -1965,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>40</v>
       </c>

</xml_diff>